<commit_message>
add not important files
</commit_message>
<xml_diff>
--- a/tests/data/test03_v1c3city_diff_time.xlsx
+++ b/tests/data/test03_v1c3city_diff_time.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://columbusglobal-my.sharepoint.com/personal/voev_columbusglobal_com/Documents/av_doc/Vehicle-Routing/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\voev\OneDrive - Columbus\av_doc\Vehicle-Routing\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="8_{1C197FCC-D555-4110-9B11-7FD88CA513E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B47293C9-07AC-484D-896C-D6C803465F20}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAC588C-381B-427D-BEC9-C0C673AE1DAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="444" yWindow="648" windowWidth="21732" windowHeight="11700" activeTab="4" xr2:uid="{A9E439BE-6E4E-4148-9B5A-691A88720DDA}"/>
+    <workbookView xWindow="804" yWindow="0" windowWidth="21732" windowHeight="11700" activeTab="5" xr2:uid="{A9E439BE-6E4E-4148-9B5A-691A88720DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="TestDescription" sheetId="7" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
   <si>
     <t>minPeriod</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Moscow</t>
   </si>
   <si>
-    <t>Tambov</t>
-  </si>
-  <si>
     <t>Voronezh</t>
   </si>
   <si>
@@ -109,7 +106,13 @@
     <t>Nissan</t>
   </si>
   <si>
-    <t>Demand in the  same city but with different time windows</t>
+    <t>Split order (city) to two with zero distnance between them</t>
+  </si>
+  <si>
+    <t>Tambov1</t>
+  </si>
+  <si>
+    <t>Tambov2</t>
   </si>
 </sst>
 </file>
@@ -146,8 +149,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,33 +468,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4233BAE-DDE8-4CE7-8712-865422E880CC}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -514,10 +516,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -543,7 +545,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2523AFC6-E9D3-42BA-B8E2-DF666CE4C56C}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -553,7 +555,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -563,12 +565,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -580,9 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A63F9D6-8E1E-47DB-A888-63391971C3C4}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -591,21 +596,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="C2">
         <v>9</v>
@@ -620,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCA095E-D3F7-49C8-BD5C-B9B8E0BE66A7}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,70 +637,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="C2">
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
       <c r="E2">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="C3">
-        <v>1100</v>
+        <v>850</v>
       </c>
       <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3">
         <v>17</v>
-      </c>
-      <c r="E3">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C4">
-        <v>900</v>
+        <v>1100</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E4">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -705,26 +710,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723586A4-2014-4229-857C-3037F57FC317}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -732,7 +737,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -746,7 +751,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -757,7 +762,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -771,10 +776,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>2.1111111111111112</v>
@@ -785,10 +790,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>2.1111111111111112</v>
@@ -799,7 +804,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -809,6 +814,118 @@
       </c>
       <c r="D7">
         <v>450</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>2.1111111111111112</v>
+      </c>
+      <c r="D11">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>2.1111111111111112</v>
+      </c>
+      <c r="D12">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>